<commit_message>
da sua quiz, question, them date
</commit_message>
<xml_diff>
--- a/web/sheet/import-quiz-template.xlsx
+++ b/web/sheet/import-quiz-template.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\CLoneCode\SWP391_G5\web\sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Code\SWP391_G5\web\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>question</t>
   </si>
@@ -51,12 +51,15 @@
   </si>
   <si>
     <t>optionCorrect</t>
+  </si>
+  <si>
+    <t>Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,26 +371,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="24.54296875" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,8 +419,16 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J14">
+      <formula1>"Math,Japanese,English,Germany,Project,Literature"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>